<commit_message>
Updated all user review data
</commit_message>
<xml_diff>
--- a/LCDP_User_Reviews/Mendix_Reviews_100.xlsx
+++ b/LCDP_User_Reviews/Mendix_Reviews_100.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IIITB-LJMU\IIITB-LJMU-Course-Material\MS Computer Science\Thesis\Low Code For Legacy Modernization Data\Mendix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ABE3C5-CA99-4DBE-A980-D909865BF6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E262CCE-8363-4874-99A0-53D4AAC43B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="212">
   <si>
-    <t>Review 2023 (last 12 months)</t>
-  </si>
-  <si>
     <t>SI</t>
   </si>
   <si>
@@ -663,13 +660,16 @@
   </si>
   <si>
     <t>Fast development, performance</t>
+  </si>
+  <si>
+    <t>Latest 100 reviews</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -677,13 +677,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -713,16 +727,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E2:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1018,22 +1029,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="F2" t="s">
-        <v>0</v>
+      <c r="F2" s="3" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="5:8" ht="72" x14ac:dyDescent="0.3">
@@ -1041,13 +1052,13 @@
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1055,13 +1066,13 @@
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1069,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.3">
@@ -1083,13 +1094,13 @@
         <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1097,13 +1108,13 @@
         <v>5</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1111,13 +1122,13 @@
         <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1125,13 +1136,13 @@
         <v>7</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.3">
@@ -1139,13 +1150,13 @@
         <v>8</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="H12" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.3">
@@ -1153,13 +1164,13 @@
         <v>9</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.3">
@@ -1167,13 +1178,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.3">
@@ -1181,13 +1192,13 @@
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.3">
@@ -1195,13 +1206,13 @@
         <v>12</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.3">
@@ -1209,13 +1220,13 @@
         <v>13</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.3">
@@ -1223,13 +1234,13 @@
         <v>14</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.3">
@@ -1237,13 +1248,13 @@
         <v>15</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1251,13 +1262,13 @@
         <v>16</v>
       </c>
       <c r="F20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H20" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.3">
@@ -1265,13 +1276,13 @@
         <v>17</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.3">
@@ -1279,13 +1290,13 @@
         <v>18</v>
       </c>
       <c r="F22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="H22" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1293,13 +1304,13 @@
         <v>19</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1307,13 +1318,13 @@
         <v>20</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1321,13 +1332,13 @@
         <v>21</v>
       </c>
       <c r="F25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="H25" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1335,13 +1346,13 @@
         <v>22</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="H26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1349,13 +1360,13 @@
         <v>23</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="H27" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="5:8" x14ac:dyDescent="0.3">
@@ -1363,13 +1374,13 @@
         <v>24</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="5:8" x14ac:dyDescent="0.3">
@@ -1377,13 +1388,13 @@
         <v>25</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1391,13 +1402,13 @@
         <v>26</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="H30" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="5:8" x14ac:dyDescent="0.3">
@@ -1405,13 +1416,13 @@
         <v>27</v>
       </c>
       <c r="F31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="H31" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1419,13 +1430,13 @@
         <v>28</v>
       </c>
       <c r="F32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="H32" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="5:8" x14ac:dyDescent="0.3">
@@ -1433,13 +1444,13 @@
         <v>29</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1447,13 +1458,13 @@
         <v>30</v>
       </c>
       <c r="F34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G34" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="H34" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1461,13 +1472,13 @@
         <v>31</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1475,13 +1486,13 @@
         <v>32</v>
       </c>
       <c r="F36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1489,13 +1500,13 @@
         <v>33</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="5:8" x14ac:dyDescent="0.3">
@@ -1503,13 +1514,13 @@
         <v>34</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="H38" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="5:8" x14ac:dyDescent="0.3">
@@ -1517,13 +1528,13 @@
         <v>35</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="5:8" x14ac:dyDescent="0.3">
@@ -1531,13 +1542,13 @@
         <v>36</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="5:8" x14ac:dyDescent="0.3">
@@ -1545,13 +1556,13 @@
         <v>37</v>
       </c>
       <c r="F41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="H41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42" spans="5:8" x14ac:dyDescent="0.3">
@@ -1559,13 +1570,13 @@
         <v>38</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="H42" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="5:8" x14ac:dyDescent="0.3">
@@ -1573,13 +1584,13 @@
         <v>39</v>
       </c>
       <c r="F43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="H43" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="5:8" x14ac:dyDescent="0.3">
@@ -1587,13 +1598,13 @@
         <v>40</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G44" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="H44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1601,13 +1612,13 @@
         <v>41</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1615,13 +1626,13 @@
         <v>42</v>
       </c>
       <c r="F46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="H46" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="5:8" x14ac:dyDescent="0.3">
@@ -1629,13 +1640,13 @@
         <v>43</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="5:8" x14ac:dyDescent="0.3">
@@ -1643,13 +1654,13 @@
         <v>44</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.3">
@@ -1657,13 +1668,13 @@
         <v>45</v>
       </c>
       <c r="F49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G49" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="H49" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.3">
@@ -1671,13 +1682,13 @@
         <v>46</v>
       </c>
       <c r="F50" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1685,13 +1696,13 @@
         <v>47</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G51" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.3">
@@ -1699,13 +1710,13 @@
         <v>48</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.3">
@@ -1713,13 +1724,13 @@
         <v>49</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.3">
@@ -1727,13 +1738,13 @@
         <v>50</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1741,13 +1752,13 @@
         <v>51</v>
       </c>
       <c r="F55" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G55" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="H55" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.3">
@@ -1755,13 +1766,13 @@
         <v>52</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.3">
@@ -1769,13 +1780,13 @@
         <v>53</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1783,13 +1794,13 @@
         <v>54</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.3">
@@ -1797,13 +1808,13 @@
         <v>55</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1811,13 +1822,13 @@
         <v>56</v>
       </c>
       <c r="F60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G60" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="H60" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.3">
@@ -1825,13 +1836,13 @@
         <v>57</v>
       </c>
       <c r="F61" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G61" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G61" s="1" t="s">
-        <v>113</v>
-      </c>
       <c r="H61" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1839,13 +1850,13 @@
         <v>58</v>
       </c>
       <c r="F62" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="G62" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G62" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="H62" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="5:8" ht="259.2" x14ac:dyDescent="0.3">
@@ -1853,13 +1864,13 @@
         <v>59</v>
       </c>
       <c r="F63" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G63" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="G63" s="1" t="s">
+      <c r="H63" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="64" spans="5:8" x14ac:dyDescent="0.3">
@@ -1867,13 +1878,13 @@
         <v>60</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -1881,13 +1892,13 @@
         <v>61</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="5:8" ht="72" x14ac:dyDescent="0.3">
@@ -1895,13 +1906,13 @@
         <v>62</v>
       </c>
       <c r="F66" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="67" spans="5:8" ht="129.6" x14ac:dyDescent="0.3">
@@ -1909,531 +1920,531 @@
         <v>63</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>128</v>
-      </c>
     </row>
     <row r="68" spans="5:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="E68" s="3">
+      <c r="E68" s="1">
         <v>64</v>
       </c>
-      <c r="F68" s="4" t="s">
+      <c r="F68" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H68" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="G68" s="3" t="s">
+    </row>
+    <row r="69" spans="5:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="E69" s="1">
+        <v>65</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E70" s="1">
+        <v>66</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E71" s="1">
+        <v>67</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E72" s="1">
+        <v>68</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E73" s="1">
+        <v>69</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E74" s="1">
+        <v>70</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="5:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="E75" s="1">
+        <v>71</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="76" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E76" s="1">
+        <v>72</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E77" s="1">
+        <v>73</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E78" s="1">
+        <v>74</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E79" s="1">
         <v>75</v>
       </c>
-      <c r="H68" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="5:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="E69" s="3">
-        <v>65</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="70" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E70" s="3">
-        <v>66</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="G70" s="3" t="s">
+      <c r="F79" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E80" s="1">
+        <v>76</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="5:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E81" s="1">
+        <v>77</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="82" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E82" s="1">
+        <v>78</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E83" s="1">
+        <v>79</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E84" s="1">
+        <v>80</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H70" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="71" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E71" s="3">
-        <v>67</v>
-      </c>
-      <c r="F71" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E72" s="3">
-        <v>68</v>
-      </c>
-      <c r="F72" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E73" s="3">
-        <v>69</v>
-      </c>
-      <c r="F73" s="4" t="s">
+      <c r="G84" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E85" s="1">
+        <v>81</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E86" s="1">
+        <v>82</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E87" s="1">
+        <v>83</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="G87" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E88" s="1">
+        <v>84</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" spans="5:8" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="E89" s="1">
+        <v>85</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E90" s="1">
+        <v>86</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E91" s="1">
+        <v>87</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="5:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="E92" s="1">
+        <v>88</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="93" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E93" s="1">
+        <v>89</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E94" s="1">
+        <v>90</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H94" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E95" s="1">
+        <v>91</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="G95" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E74" s="3">
-        <v>70</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H74" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="5:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="E75" s="3">
-        <v>71</v>
-      </c>
-      <c r="F75" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="76" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E76" s="3">
-        <v>72</v>
-      </c>
-      <c r="F76" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G76" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H76" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="77" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E77" s="3">
-        <v>73</v>
-      </c>
-      <c r="F77" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H77" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="78" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E78" s="3">
-        <v>74</v>
-      </c>
-      <c r="F78" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H78" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" spans="5:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E79" s="3">
-        <v>75</v>
-      </c>
-      <c r="F79" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="80" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E80" s="3">
-        <v>76</v>
-      </c>
-      <c r="F80" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="81" spans="5:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="E81" s="3">
-        <v>77</v>
-      </c>
-      <c r="F81" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="H81" s="4" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="82" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E82" s="3">
-        <v>78</v>
-      </c>
-      <c r="F82" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H82" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E83" s="3">
-        <v>79</v>
-      </c>
-      <c r="F83" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H83" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E84" s="3">
-        <v>80</v>
-      </c>
-      <c r="F84" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G84" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H84" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="85" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E85" s="3">
-        <v>81</v>
-      </c>
-      <c r="F85" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="G85" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H85" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E86" s="3">
-        <v>82</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="G86" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H86" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E87" s="3">
-        <v>83</v>
-      </c>
-      <c r="F87" s="4" t="s">
+      <c r="H95" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E96" s="1">
+        <v>92</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="97" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E97" s="1">
+        <v>93</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H97" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="98" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E98" s="1">
+        <v>94</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H98" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E99" s="1">
+        <v>95</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E100" s="1">
+        <v>96</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E101" s="1">
+        <v>97</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="102" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E102" s="1">
+        <v>98</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G102" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H102" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="5:8" ht="144" x14ac:dyDescent="0.3">
+      <c r="E103" s="1">
+        <v>99</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="G103" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G87" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H87" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E88" s="3">
-        <v>84</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G88" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H88" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="89" spans="5:8" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="E89" s="3">
-        <v>85</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H89" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="90" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E90" s="3">
-        <v>86</v>
-      </c>
-      <c r="F90" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="91" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E91" s="3">
-        <v>87</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="H91" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="92" spans="5:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="E92" s="3">
-        <v>88</v>
-      </c>
-      <c r="F92" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="G92" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H92" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="93" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E93" s="3">
-        <v>89</v>
-      </c>
-      <c r="F93" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="G93" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="H93" s="4" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="94" spans="5:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E94" s="3">
-        <v>90</v>
-      </c>
-      <c r="F94" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="G94" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H94" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E95" s="3">
-        <v>91</v>
-      </c>
-      <c r="F95" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="G95" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H95" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E96" s="3">
-        <v>92</v>
-      </c>
-      <c r="F96" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G96" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H96" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="97" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E97" s="3">
-        <v>93</v>
-      </c>
-      <c r="F97" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H97" s="4" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="98" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E98" s="3">
-        <v>94</v>
-      </c>
-      <c r="F98" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H98" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="99" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E99" s="3">
-        <v>95</v>
-      </c>
-      <c r="F99" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="G99" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H99" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E100" s="3">
-        <v>96</v>
-      </c>
-      <c r="F100" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="G100" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="H100" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="5:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E101" s="3">
-        <v>97</v>
-      </c>
-      <c r="F101" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="102" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E102" s="3">
-        <v>98</v>
-      </c>
-      <c r="F102" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="H102" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="5:8" ht="144" x14ac:dyDescent="0.3">
-      <c r="E103" s="3">
-        <v>99</v>
-      </c>
-      <c r="F103" s="4" t="s">
+      <c r="H103" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="G103" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H103" s="4" t="s">
+    </row>
+    <row r="104" spans="5:8" x14ac:dyDescent="0.3">
+      <c r="E104" s="1">
+        <v>100</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G104" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="104" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E104" s="3">
-        <v>100</v>
-      </c>
-      <c r="F104" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>5</v>
+      <c r="H104" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>